<commit_message>
finish with result file
</commit_message>
<xml_diff>
--- a/Day 2/data.xlsx
+++ b/Day 2/data.xlsx
@@ -20,17 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="32">
   <si>
     <t>Спокойствие</t>
   </si>
   <si>
-    <t>Физическое сост.</t>
-  </si>
-  <si>
-    <t>Психологическое сост.</t>
-  </si>
-  <si>
     <t>Скорость реакции</t>
   </si>
   <si>
@@ -116,6 +110,12 @@
   </si>
   <si>
     <t>номер пилота</t>
+  </si>
+  <si>
+    <t>Физическое состояние</t>
+  </si>
+  <si>
+    <t>Психологическое состояние</t>
   </si>
 </sst>
 </file>
@@ -152,8 +152,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -458,7 +459,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -471,22 +472,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -494,7 +495,7 @@
         <v>90.6</v>
       </c>
       <c r="B2">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="C2">
         <v>55</v>
@@ -519,47 +520,50 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:L2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1">
+        <v>42736</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -620,45 +624,45 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>22.6</v>
@@ -699,7 +703,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>32.6</v>
@@ -740,7 +744,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>42.6</v>
@@ -781,7 +785,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>52.6</v>
@@ -822,7 +826,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>62.6</v>
@@ -882,45 +886,45 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2">
         <v>22.6</v>
@@ -961,7 +965,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>32.6</v>
@@ -1017,45 +1021,45 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>22.6</v>
@@ -1096,7 +1100,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>32.6</v>
@@ -1152,45 +1156,45 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2">
         <v>22.6</v>
@@ -1231,7 +1235,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>32.6</v>
@@ -1272,7 +1276,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>42.6</v>
@@ -1313,7 +1317,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>52.6</v>
@@ -1359,10 +1363,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:B2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1370,13 +1374,13 @@
     <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>123</v>
       </c>
     </row>

</xml_diff>